<commit_message>
repair application after tg session config was lost
</commit_message>
<xml_diff>
--- a/SocialNetworkAnalyzer/Analytics.xlsx
+++ b/SocialNetworkAnalyzer/Analytics.xlsx
@@ -472,7 +472,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J290"/>
+  <dimension ref="A1:J301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11006,6 +11006,398 @@
         <v>0</v>
       </c>
     </row>
+    <row r="291">
+      <c r="A291" s="7" t="n"/>
+      <c r="B291" s="7" t="n"/>
+      <c r="C291" s="7" t="n"/>
+      <c r="D291" s="7" t="n"/>
+      <c r="E291" s="7" t="n"/>
+      <c r="F291" s="7" t="n"/>
+      <c r="G291" s="7" t="n"/>
+      <c r="H291" s="7" t="n"/>
+      <c r="I291" s="7" t="n"/>
+      <c r="J291" s="7" t="n"/>
+    </row>
+    <row r="292">
+      <c r="A292" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B292" t="inlineStr">
+        <is>
+          <t>После длительного использования телефон часто...</t>
+        </is>
+      </c>
+      <c r="C292" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3410</t>
+        </is>
+      </c>
+      <c r="D292" t="n">
+        <v>139</v>
+      </c>
+      <c r="E292" t="n">
+        <v>0</v>
+      </c>
+      <c r="F292" t="n">
+        <v>10</v>
+      </c>
+      <c r="G292" t="n">
+        <v>0</v>
+      </c>
+      <c r="H292" s="8" t="n">
+        <v>85</v>
+      </c>
+      <c r="I292" t="n">
+        <v>5102</v>
+      </c>
+      <c r="J292" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="293">
+      <c r="A293" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B293" t="inlineStr">
+        <is>
+          <t>Творожный сыр воспринимается как полезный...</t>
+        </is>
+      </c>
+      <c r="C293" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3416</t>
+        </is>
+      </c>
+      <c r="D293" t="n">
+        <v>100</v>
+      </c>
+      <c r="E293" t="n">
+        <v>1</v>
+      </c>
+      <c r="F293" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G293" t="n">
+        <v>0</v>
+      </c>
+      <c r="H293" t="n">
+        <v>31</v>
+      </c>
+      <c r="I293" t="n">
+        <v>5441</v>
+      </c>
+      <c r="J293" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B294" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Сегодня отмечается Всемирный день яйца..</t>
+        </is>
+      </c>
+      <c r="C294" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3418</t>
+        </is>
+      </c>
+      <c r="D294" s="9" t="n">
+        <v>53</v>
+      </c>
+      <c r="E294" t="n">
+        <v>0</v>
+      </c>
+      <c r="F294" t="n">
+        <v>3</v>
+      </c>
+      <c r="G294" t="n">
+        <v>0</v>
+      </c>
+      <c r="H294" t="n">
+        <v>12</v>
+      </c>
+      <c r="I294" s="9" t="n">
+        <v>5023</v>
+      </c>
+      <c r="J294" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B295" t="inlineStr">
+        <is>
+          <t>Почему некоторые яйца плохо...</t>
+        </is>
+      </c>
+      <c r="C295" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3420</t>
+        </is>
+      </c>
+      <c r="D295" t="n">
+        <v>76</v>
+      </c>
+      <c r="E295" t="n">
+        <v>0</v>
+      </c>
+      <c r="F295" t="n">
+        <v>6</v>
+      </c>
+      <c r="G295" t="n">
+        <v>0</v>
+      </c>
+      <c r="H295" t="n">
+        <v>15</v>
+      </c>
+      <c r="I295" t="n">
+        <v>5165</v>
+      </c>
+      <c r="J295" t="n">
+        <v>2414</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B296" t="inlineStr">
+        <is>
+          <t>Коричневые яйца вкуснее и полезнее...</t>
+        </is>
+      </c>
+      <c r="C296" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3421</t>
+        </is>
+      </c>
+      <c r="D296" t="n">
+        <v>57</v>
+      </c>
+      <c r="E296" t="n">
+        <v>0</v>
+      </c>
+      <c r="F296" t="n">
+        <v>2</v>
+      </c>
+      <c r="G296" t="n">
+        <v>0</v>
+      </c>
+      <c r="H296" t="n">
+        <v>5</v>
+      </c>
+      <c r="I296" t="n">
+        <v>5633</v>
+      </c>
+      <c r="J296" t="n">
+        <v>2443</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B297" t="inlineStr">
+        <is>
+          <t>Крупные яйца вкуснее и полезнее...</t>
+        </is>
+      </c>
+      <c r="C297" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3422</t>
+        </is>
+      </c>
+      <c r="D297" t="n">
+        <v>56</v>
+      </c>
+      <c r="E297" t="n">
+        <v>0</v>
+      </c>
+      <c r="F297" t="n">
+        <v>2</v>
+      </c>
+      <c r="G297" t="n">
+        <v>0</v>
+      </c>
+      <c r="H297" t="n">
+        <v>6</v>
+      </c>
+      <c r="I297" t="n">
+        <v>5658</v>
+      </c>
+      <c r="J297" t="n">
+        <v>2463</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B298" t="inlineStr">
+        <is>
+          <t>Что означает буква «С» на упаковке...</t>
+        </is>
+      </c>
+      <c r="C298" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3423</t>
+        </is>
+      </c>
+      <c r="D298" t="n">
+        <v>69</v>
+      </c>
+      <c r="E298" t="n">
+        <v>0</v>
+      </c>
+      <c r="F298" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="G298" t="n">
+        <v>0</v>
+      </c>
+      <c r="H298" t="n">
+        <v>8</v>
+      </c>
+      <c r="I298" t="n">
+        <v>5334</v>
+      </c>
+      <c r="J298" s="8" t="n">
+        <v>2537</v>
+      </c>
+    </row>
+    <row r="299">
+      <c r="A299" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B299" t="inlineStr">
+        <is>
+          <t>Сегодня отмечает день рождения руководитель...</t>
+        </is>
+      </c>
+      <c r="C299" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3424</t>
+        </is>
+      </c>
+      <c r="D299" s="8" t="n">
+        <v>202</v>
+      </c>
+      <c r="E299" s="8" t="n">
+        <v>6</v>
+      </c>
+      <c r="F299" t="n">
+        <v>4</v>
+      </c>
+      <c r="G299" t="n">
+        <v>0</v>
+      </c>
+      <c r="H299" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="I299" t="n">
+        <v>5546</v>
+      </c>
+      <c r="J299" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B300" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Друзья! Совсем скоро весь мир будет отмечать...</t>
+        </is>
+      </c>
+      <c r="C300" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3425</t>
+        </is>
+      </c>
+      <c r="D300" t="n">
+        <v>92</v>
+      </c>
+      <c r="E300" t="n">
+        <v>0</v>
+      </c>
+      <c r="F300" t="n">
+        <v>5</v>
+      </c>
+      <c r="G300" t="n">
+        <v>0</v>
+      </c>
+      <c r="H300" t="n">
+        <v>4</v>
+      </c>
+      <c r="I300" t="n">
+        <v>5586</v>
+      </c>
+      <c r="J300" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B301" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Выбираем в магазине качественную томатную...</t>
+        </is>
+      </c>
+      <c r="C301" t="inlineStr">
+        <is>
+          <t>https://t.me/RSKRFRU/3426</t>
+        </is>
+      </c>
+      <c r="D301" t="n">
+        <v>116</v>
+      </c>
+      <c r="E301" t="n">
+        <v>0</v>
+      </c>
+      <c r="F301" t="n">
+        <v>6</v>
+      </c>
+      <c r="G301" t="n">
+        <v>0</v>
+      </c>
+      <c r="H301" t="n">
+        <v>19</v>
+      </c>
+      <c r="I301" s="8" t="n">
+        <v>6064</v>
+      </c>
+      <c r="J301" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" paperSize="9"/>
@@ -11018,7 +11410,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I307"/>
+  <dimension ref="A1:I325"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:I1"/>
@@ -21309,6 +21701,612 @@
         <v>18</v>
       </c>
     </row>
+    <row r="308">
+      <c r="A308" s="7" t="n"/>
+      <c r="B308" s="7" t="n"/>
+      <c r="C308" s="7" t="n"/>
+      <c r="D308" s="7" t="n"/>
+      <c r="E308" s="7" t="n"/>
+      <c r="F308" s="7" t="n"/>
+      <c r="G308" s="7" t="n"/>
+      <c r="H308" s="7" t="n"/>
+      <c r="I308" s="7" t="n"/>
+    </row>
+    <row r="309">
+      <c r="A309" t="inlineStr">
+        <is>
+          <t>06.10.2023</t>
+        </is>
+      </c>
+      <c r="B309" t="inlineStr">
+        <is>
+          <t>Что обнаружили в томатной пасте?На полках магази</t>
+        </is>
+      </c>
+      <c r="C309" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_179789</t>
+        </is>
+      </c>
+      <c r="D309" t="n">
+        <v>173</v>
+      </c>
+      <c r="E309" t="n">
+        <v>165</v>
+      </c>
+      <c r="F309" t="n">
+        <v>25</v>
+      </c>
+      <c r="G309" t="n">
+        <v>12418</v>
+      </c>
+      <c r="H309" t="n">
+        <v>1</v>
+      </c>
+      <c r="I309" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" t="inlineStr">
+        <is>
+          <t>07.10.2023</t>
+        </is>
+      </c>
+      <c r="B310" t="inlineStr">
+        <is>
+          <t>Инвалиды имеют ряд льгот, в том числе в области во</t>
+        </is>
+      </c>
+      <c r="C310" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_179948</t>
+        </is>
+      </c>
+      <c r="D310" t="n">
+        <v>109</v>
+      </c>
+      <c r="E310" s="9" t="n">
+        <v>72</v>
+      </c>
+      <c r="F310" t="n">
+        <v>18</v>
+      </c>
+      <c r="G310" t="n">
+        <v>11360</v>
+      </c>
+      <c r="H310" t="n">
+        <v>0</v>
+      </c>
+      <c r="I310" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>08.10.2023</t>
+        </is>
+      </c>
+      <c r="B311" t="inlineStr">
+        <is>
+          <t>Двухфакторная аутентификация на Госуслугах стала о</t>
+        </is>
+      </c>
+      <c r="C311" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_180050</t>
+        </is>
+      </c>
+      <c r="D311" t="n">
+        <v>195</v>
+      </c>
+      <c r="E311" t="n">
+        <v>89</v>
+      </c>
+      <c r="F311" t="n">
+        <v>91</v>
+      </c>
+      <c r="G311" t="n">
+        <v>15184</v>
+      </c>
+      <c r="H311" t="n">
+        <v>0</v>
+      </c>
+      <c r="I311" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B312" t="inlineStr">
+        <is>
+          <t>Из-за испарения воды высушенный кусочек фрукта сил</t>
+        </is>
+      </c>
+      <c r="C312" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_180165</t>
+        </is>
+      </c>
+      <c r="D312" t="n">
+        <v>327</v>
+      </c>
+      <c r="E312" t="n">
+        <v>271</v>
+      </c>
+      <c r="F312" t="n">
+        <v>115</v>
+      </c>
+      <c r="G312" t="n">
+        <v>29609</v>
+      </c>
+      <c r="H312" t="n">
+        <v>0</v>
+      </c>
+      <c r="I312" t="n">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B313" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Стоит ли бояться нитратов и нитритов? Это один из </t>
+        </is>
+      </c>
+      <c r="C313" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_180280</t>
+        </is>
+      </c>
+      <c r="D313" t="n">
+        <v>298</v>
+      </c>
+      <c r="E313" t="n">
+        <v>154</v>
+      </c>
+      <c r="F313" t="n">
+        <v>96</v>
+      </c>
+      <c r="G313" t="n">
+        <v>25099</v>
+      </c>
+      <c r="H313" t="n">
+        <v>2</v>
+      </c>
+      <c r="I313" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B314" t="inlineStr">
+        <is>
+          <t>Говяжья печень является уникальным продуктом, поск</t>
+        </is>
+      </c>
+      <c r="C314" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_180590</t>
+        </is>
+      </c>
+      <c r="D314" t="n">
+        <v>234</v>
+      </c>
+      <c r="E314" t="n">
+        <v>274</v>
+      </c>
+      <c r="F314" t="n">
+        <v>80</v>
+      </c>
+      <c r="G314" t="n">
+        <v>18051</v>
+      </c>
+      <c r="H314" t="n">
+        <v>1</v>
+      </c>
+      <c r="I314" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="315">
+      <c r="A315" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B315" t="inlineStr">
+        <is>
+          <t>Друзья! Заметили ли вы, что за последний год на по</t>
+        </is>
+      </c>
+      <c r="C315" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_180655</t>
+        </is>
+      </c>
+      <c r="D315" s="9" t="n">
+        <v>93</v>
+      </c>
+      <c r="E315" t="n">
+        <v>205</v>
+      </c>
+      <c r="F315" t="n">
+        <v>2</v>
+      </c>
+      <c r="G315" t="n">
+        <v>13413</v>
+      </c>
+      <c r="H315" t="n">
+        <v>1</v>
+      </c>
+      <c r="I315" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B316" t="inlineStr">
+        <is>
+          <t>Псевдокоммунальщики могут делать поквартирный обхо</t>
+        </is>
+      </c>
+      <c r="C316" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181082</t>
+        </is>
+      </c>
+      <c r="D316" t="n">
+        <v>216</v>
+      </c>
+      <c r="E316" t="n">
+        <v>194</v>
+      </c>
+      <c r="F316" t="n">
+        <v>86</v>
+      </c>
+      <c r="G316" t="n">
+        <v>20903</v>
+      </c>
+      <c r="H316" t="n">
+        <v>1</v>
+      </c>
+      <c r="I316" t="n">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B317" t="inlineStr">
+        <is>
+          <t>Мы постоянно слышим, что для здоровья и фигуры пол</t>
+        </is>
+      </c>
+      <c r="C317" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181201</t>
+        </is>
+      </c>
+      <c r="D317" s="8" t="n">
+        <v>513</v>
+      </c>
+      <c r="E317" s="8" t="n">
+        <v>288</v>
+      </c>
+      <c r="F317" s="8" t="n">
+        <v>279</v>
+      </c>
+      <c r="G317" s="8" t="n">
+        <v>37710</v>
+      </c>
+      <c r="H317" t="n">
+        <v>4</v>
+      </c>
+      <c r="I317" s="8" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B318" t="inlineStr">
+        <is>
+          <t>Роскачество вышло на рынок строительного оборудова</t>
+        </is>
+      </c>
+      <c r="C318" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181522</t>
+        </is>
+      </c>
+      <c r="D318" t="n">
+        <v>110</v>
+      </c>
+      <c r="E318" t="n">
+        <v>112</v>
+      </c>
+      <c r="F318" t="n">
+        <v>18</v>
+      </c>
+      <c r="G318" t="n">
+        <v>6904</v>
+      </c>
+      <c r="H318" t="n">
+        <v>0</v>
+      </c>
+      <c r="I318" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B319" t="inlineStr">
+        <is>
+          <t>Совсем скоро придет время навести порядок в гардер</t>
+        </is>
+      </c>
+      <c r="C319" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181616</t>
+        </is>
+      </c>
+      <c r="D319" t="n">
+        <v>198</v>
+      </c>
+      <c r="E319" t="n">
+        <v>226</v>
+      </c>
+      <c r="F319" t="n">
+        <v>47</v>
+      </c>
+      <c r="G319" t="n">
+        <v>8594</v>
+      </c>
+      <c r="H319" t="n">
+        <v>0</v>
+      </c>
+      <c r="I319" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B320" t="inlineStr">
+        <is>
+          <t>Театральный сезон уже начался: новые спектакли пре</t>
+        </is>
+      </c>
+      <c r="C320" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181792</t>
+        </is>
+      </c>
+      <c r="D320" t="n">
+        <v>148</v>
+      </c>
+      <c r="E320" t="n">
+        <v>157</v>
+      </c>
+      <c r="F320" t="n">
+        <v>10</v>
+      </c>
+      <c r="G320" t="n">
+        <v>24506</v>
+      </c>
+      <c r="H320" t="n">
+        <v>4</v>
+      </c>
+      <c r="I320" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="321">
+      <c r="A321" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B321" t="inlineStr">
+        <is>
+          <t>После длительного использования телефон часто начи</t>
+        </is>
+      </c>
+      <c r="C321" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_181989</t>
+        </is>
+      </c>
+      <c r="D321" t="n">
+        <v>251</v>
+      </c>
+      <c r="E321" t="n">
+        <v>158</v>
+      </c>
+      <c r="F321" t="n">
+        <v>131</v>
+      </c>
+      <c r="G321" t="n">
+        <v>10221</v>
+      </c>
+      <c r="H321" t="n">
+        <v>0</v>
+      </c>
+      <c r="I321" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B322" t="inlineStr">
+        <is>
+          <t>Творожный сыр воспринимается как полезный продукт,</t>
+        </is>
+      </c>
+      <c r="C322" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_182158</t>
+        </is>
+      </c>
+      <c r="D322" t="n">
+        <v>139</v>
+      </c>
+      <c r="E322" t="n">
+        <v>197</v>
+      </c>
+      <c r="F322" t="n">
+        <v>26</v>
+      </c>
+      <c r="G322" t="n">
+        <v>9495</v>
+      </c>
+      <c r="H322" t="n">
+        <v>1</v>
+      </c>
+      <c r="I322" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B323" t="inlineStr">
+        <is>
+          <t>Сегодня отмечает день рождения руководитель Роска</t>
+        </is>
+      </c>
+      <c r="C323" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_182319</t>
+        </is>
+      </c>
+      <c r="D323" t="n">
+        <v>157</v>
+      </c>
+      <c r="E323" t="n">
+        <v>85</v>
+      </c>
+      <c r="F323" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G323" s="9" t="n">
+        <v>6795</v>
+      </c>
+      <c r="H323" t="n">
+        <v>1</v>
+      </c>
+      <c r="I323" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B324" t="inlineStr">
+        <is>
+          <t>Друзья! Совсем скоро весь мир будет отмечать Всеми</t>
+        </is>
+      </c>
+      <c r="C324" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_182369</t>
+        </is>
+      </c>
+      <c r="D324" t="n">
+        <v>143</v>
+      </c>
+      <c r="E324" t="n">
+        <v>193</v>
+      </c>
+      <c r="F324" t="n">
+        <v>9</v>
+      </c>
+      <c r="G324" t="n">
+        <v>8238</v>
+      </c>
+      <c r="H324" t="n">
+        <v>2</v>
+      </c>
+      <c r="I324" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B325" t="inlineStr">
+        <is>
+          <t>Выбираем в магазине качественную томатную пасту, о</t>
+        </is>
+      </c>
+      <c r="C325" t="inlineStr">
+        <is>
+          <t>https://vk.com/rskrf?w=wall-94833853_182555</t>
+        </is>
+      </c>
+      <c r="D325" t="n">
+        <v>145</v>
+      </c>
+      <c r="E325" t="n">
+        <v>126</v>
+      </c>
+      <c r="F325" t="n">
+        <v>6</v>
+      </c>
+      <c r="G325" t="n">
+        <v>8244</v>
+      </c>
+      <c r="H325" t="n">
+        <v>4</v>
+      </c>
+      <c r="I325" t="n">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -21320,7 +22318,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G251"/>
+  <dimension ref="A1:G289"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:G1"/>
@@ -28219,6 +29217,1088 @@
         <v>3323</v>
       </c>
     </row>
+    <row r="252">
+      <c r="A252" s="7" t="n"/>
+      <c r="B252" s="7" t="n"/>
+      <c r="C252" s="7" t="n"/>
+      <c r="D252" s="7" t="n"/>
+      <c r="E252" s="7" t="n"/>
+      <c r="F252" s="7" t="n"/>
+      <c r="G252" s="7" t="n"/>
+    </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>25.09.2023</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>Друзья! Мы запускаем конкурс совместно с...</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156930017407021</t>
+        </is>
+      </c>
+      <c r="D253" s="8" t="n">
+        <v>224</v>
+      </c>
+      <c r="E253" s="8" t="n">
+        <v>525</v>
+      </c>
+      <c r="F253" s="8" t="n">
+        <v>84</v>
+      </c>
+      <c r="G253" s="8" t="n">
+        <v>56769</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>25.09.2023</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Интернет полнится мифами из мира цифровых...</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156930691641389</t>
+        </is>
+      </c>
+      <c r="D254" t="n">
+        <v>27</v>
+      </c>
+      <c r="E254" t="n">
+        <v>3</v>
+      </c>
+      <c r="F254" t="n">
+        <v>4</v>
+      </c>
+      <c r="G254" t="n">
+        <v>5060</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>26.09.2023</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>Температура тела может повышаться из-за болезней,...</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156933486686253</t>
+        </is>
+      </c>
+      <c r="D255" t="n">
+        <v>127</v>
+      </c>
+      <c r="E255" t="n">
+        <v>25</v>
+      </c>
+      <c r="F255" t="n">
+        <v>27</v>
+      </c>
+      <c r="G255" t="n">
+        <v>10283</v>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>26.09.2023</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>С плохой кредитной историей вам вряд ли дадут...</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156934536245293</t>
+        </is>
+      </c>
+      <c r="D256" t="n">
+        <v>14</v>
+      </c>
+      <c r="E256" t="n">
+        <v>1</v>
+      </c>
+      <c r="F256" t="n">
+        <v>2</v>
+      </c>
+      <c r="G256" t="n">
+        <v>7736</v>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>27.09.2023</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>«Потоп в квартире» из-за проблем у соседей —...</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156937252319277</t>
+        </is>
+      </c>
+      <c r="D257" t="n">
+        <v>57</v>
+      </c>
+      <c r="E257" t="n">
+        <v>3</v>
+      </c>
+      <c r="F257" t="n">
+        <v>13</v>
+      </c>
+      <c r="G257" t="n">
+        <v>6302</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>27.09.2023</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>Чтобы отслеживать ситуацию по улучшению качества...</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156937716314157</t>
+        </is>
+      </c>
+      <c r="D258" t="n">
+        <v>52</v>
+      </c>
+      <c r="E258" t="n">
+        <v>24</v>
+      </c>
+      <c r="F258" t="n">
+        <v>2</v>
+      </c>
+      <c r="G258" t="n">
+        <v>8990</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>28.09.2023</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>Наиболее популярная разновидность белого хлеба –...</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156940750106669</t>
+        </is>
+      </c>
+      <c r="D259" t="n">
+        <v>36</v>
+      </c>
+      <c r="E259" t="n">
+        <v>33</v>
+      </c>
+      <c r="F259" t="n">
+        <v>5</v>
+      </c>
+      <c r="G259" t="n">
+        <v>5705</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>28.09.2023</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>Продолжаем рассказывать про уловки продавцов в...</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156941244837933</t>
+        </is>
+      </c>
+      <c r="D260" t="n">
+        <v>54</v>
+      </c>
+      <c r="E260" t="n">
+        <v>3</v>
+      </c>
+      <c r="F260" t="n">
+        <v>6</v>
+      </c>
+      <c r="G260" t="n">
+        <v>7795</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>29.09.2023</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>Самая масштабная проверка цифровой грамотности в...</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156944000167981</t>
+        </is>
+      </c>
+      <c r="D261" t="n">
+        <v>18</v>
+      </c>
+      <c r="E261" t="n">
+        <v>1</v>
+      </c>
+      <c r="F261" t="n">
+        <v>1</v>
+      </c>
+      <c r="G261" t="n">
+        <v>4171</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>29.09.2023</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>Отмечаем День бутерброда и готовим бутерброды из...</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156944379490349</t>
+        </is>
+      </c>
+      <c r="D262" t="n">
+        <v>41</v>
+      </c>
+      <c r="E262" t="n">
+        <v>7</v>
+      </c>
+      <c r="F262" t="n">
+        <v>3</v>
+      </c>
+      <c r="G262" t="n">
+        <v>4906</v>
+      </c>
+    </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>30.09.2023</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>В кулинарии сушеный чеснок используется в...</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156948057108525</t>
+        </is>
+      </c>
+      <c r="D263" t="n">
+        <v>63</v>
+      </c>
+      <c r="E263" t="n">
+        <v>7</v>
+      </c>
+      <c r="F263" t="n">
+        <v>7</v>
+      </c>
+      <c r="G263" t="n">
+        <v>5411</v>
+      </c>
+    </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>01.10.2023</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>Новый выпуск "Анатомии качества" уже доступен для...</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156951772672045</t>
+        </is>
+      </c>
+      <c r="D264" t="n">
+        <v>27</v>
+      </c>
+      <c r="E264" t="n">
+        <v>6</v>
+      </c>
+      <c r="F264" t="n">
+        <v>4</v>
+      </c>
+      <c r="G264" t="n">
+        <v>4003</v>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>02.10.2023</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>Существуют разные способы тепловой обработки —...</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156955121496109</t>
+        </is>
+      </c>
+      <c r="D265" t="n">
+        <v>127</v>
+      </c>
+      <c r="E265" t="n">
+        <v>20</v>
+      </c>
+      <c r="F265" t="n">
+        <v>31</v>
+      </c>
+      <c r="G265" t="n">
+        <v>12036</v>
+      </c>
+    </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>02.10.2023</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>От фишинга до нейросетей — у мошенников обширный...</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156955577626669</t>
+        </is>
+      </c>
+      <c r="D266" t="n">
+        <v>54</v>
+      </c>
+      <c r="E266" t="n">
+        <v>16</v>
+      </c>
+      <c r="F266" t="n">
+        <v>23</v>
+      </c>
+      <c r="G266" t="n">
+        <v>6189</v>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>Потребители часто спрашивают, откуда взялась эта...</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156958743015469</t>
+        </is>
+      </c>
+      <c r="D267" t="n">
+        <v>97</v>
+      </c>
+      <c r="E267" t="n">
+        <v>6</v>
+      </c>
+      <c r="F267" t="n">
+        <v>24</v>
+      </c>
+      <c r="G267" t="n">
+        <v>7560</v>
+      </c>
+    </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>Кредитные каникулы – это мера поддержки...</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156960176877613</t>
+        </is>
+      </c>
+      <c r="D268" s="9" t="n">
+        <v>7</v>
+      </c>
+      <c r="E268" t="n">
+        <v>1</v>
+      </c>
+      <c r="F268" t="n">
+        <v>1</v>
+      </c>
+      <c r="G268" t="n">
+        <v>2656</v>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>04.10.2023</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>Новый месяц – новый регион нашей страны со Знаком...</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156962262036525</t>
+        </is>
+      </c>
+      <c r="D269" t="n">
+        <v>55</v>
+      </c>
+      <c r="E269" t="n">
+        <v>13</v>
+      </c>
+      <c r="F269" t="n">
+        <v>8</v>
+      </c>
+      <c r="G269" t="n">
+        <v>6944</v>
+      </c>
+    </row>
+    <row r="270">
+      <c r="A270" t="inlineStr">
+        <is>
+          <t>04.10.2023</t>
+        </is>
+      </c>
+      <c r="B270" t="inlineStr">
+        <is>
+          <t>На прошлой неделе мы опубликовали новое...</t>
+        </is>
+      </c>
+      <c r="C270" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156962660626477</t>
+        </is>
+      </c>
+      <c r="D270" t="n">
+        <v>58</v>
+      </c>
+      <c r="E270" t="n">
+        <v>4</v>
+      </c>
+      <c r="F270" t="n">
+        <v>6</v>
+      </c>
+      <c r="G270" t="n">
+        <v>14809</v>
+      </c>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>05.10.2023</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t>Центр цифровой экспертизы Роскачества...</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156965423493165</t>
+        </is>
+      </c>
+      <c r="D271" t="n">
+        <v>28</v>
+      </c>
+      <c r="E271" t="n">
+        <v>1</v>
+      </c>
+      <c r="F271" t="n">
+        <v>2</v>
+      </c>
+      <c r="G271" t="n">
+        <v>5008</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>05.10.2023</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>Функциональность приложений по вызову такси...</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156965892796461</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>23</v>
+      </c>
+      <c r="E272" t="n">
+        <v>2</v>
+      </c>
+      <c r="F272" t="n">
+        <v>2</v>
+      </c>
+      <c r="G272" t="n">
+        <v>17245</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>06.10.2023</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>«Халяль» – актуальная категория внутри...</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156969216061485</t>
+        </is>
+      </c>
+      <c r="D273" t="n">
+        <v>36</v>
+      </c>
+      <c r="E273" t="n">
+        <v>14</v>
+      </c>
+      <c r="F273" t="n">
+        <v>5</v>
+      </c>
+      <c r="G273" t="n">
+        <v>11640</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>06.10.2023</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Что обнаружили в томатной пасте?...</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156970224136237</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>35</v>
+      </c>
+      <c r="E274" t="n">
+        <v>4</v>
+      </c>
+      <c r="F274" t="n">
+        <v>3</v>
+      </c>
+      <c r="G274" t="n">
+        <v>3415</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>07.10.2023</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>Инвалиды имеют ряд льгот, в том числе в области...</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156972873887789</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>17</v>
+      </c>
+      <c r="E275" t="n">
+        <v>5</v>
+      </c>
+      <c r="F275" t="n">
+        <v>5</v>
+      </c>
+      <c r="G275" t="n">
+        <v>2968</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>07.10.2023</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>Осень – время уютных вечеров, разноцветной...</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156973332967469</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>51</v>
+      </c>
+      <c r="E276" t="n">
+        <v>11</v>
+      </c>
+      <c r="F276" t="n">
+        <v>8</v>
+      </c>
+      <c r="G276" t="n">
+        <v>7472</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>08.10.2023</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>Двухфакторная аутентификация на Госуслугах стала...</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156976437407789</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>43</v>
+      </c>
+      <c r="E277" t="n">
+        <v>6</v>
+      </c>
+      <c r="F277" t="n">
+        <v>11</v>
+      </c>
+      <c r="G277" t="n">
+        <v>6758</v>
+      </c>
+    </row>
+    <row r="278">
+      <c r="A278" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B278" t="inlineStr">
+        <is>
+          <t>Из-за испарения воды высушенный кусочек фрукта...</t>
+        </is>
+      </c>
+      <c r="C278" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156979945353261</t>
+        </is>
+      </c>
+      <c r="D278" t="n">
+        <v>70</v>
+      </c>
+      <c r="E278" t="n">
+        <v>19</v>
+      </c>
+      <c r="F278" t="n">
+        <v>16</v>
+      </c>
+      <c r="G278" t="n">
+        <v>7368</v>
+      </c>
+    </row>
+    <row r="279">
+      <c r="A279" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B279" t="inlineStr">
+        <is>
+          <t>Стоит ли бояться нитратов и нитритов? Это один из...</t>
+        </is>
+      </c>
+      <c r="C279" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156980396372013</t>
+        </is>
+      </c>
+      <c r="D279" t="n">
+        <v>68</v>
+      </c>
+      <c r="E279" t="n">
+        <v>13</v>
+      </c>
+      <c r="F279" t="n">
+        <v>15</v>
+      </c>
+      <c r="G279" t="n">
+        <v>5478</v>
+      </c>
+    </row>
+    <row r="280">
+      <c r="A280" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B280" t="inlineStr">
+        <is>
+          <t>Говяжья печень является уникальным продуктом,...</t>
+        </is>
+      </c>
+      <c r="C280" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156983406899245</t>
+        </is>
+      </c>
+      <c r="D280" t="n">
+        <v>51</v>
+      </c>
+      <c r="E280" t="n">
+        <v>16</v>
+      </c>
+      <c r="F280" t="n">
+        <v>5</v>
+      </c>
+      <c r="G280" t="n">
+        <v>14840</v>
+      </c>
+    </row>
+    <row r="281">
+      <c r="A281" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B281" t="inlineStr">
+        <is>
+          <t>Псевдокоммунальщики могут делать поквартирный...</t>
+        </is>
+      </c>
+      <c r="C281" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156986876309549</t>
+        </is>
+      </c>
+      <c r="D281" t="n">
+        <v>66</v>
+      </c>
+      <c r="E281" t="n">
+        <v>6</v>
+      </c>
+      <c r="F281" t="n">
+        <v>17</v>
+      </c>
+      <c r="G281" t="n">
+        <v>7258</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B282" t="inlineStr">
+        <is>
+          <t>Мы постоянно слышим, что для здоровья и фигуры...</t>
+        </is>
+      </c>
+      <c r="C282" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156987441819693</t>
+        </is>
+      </c>
+      <c r="D282" t="n">
+        <v>91</v>
+      </c>
+      <c r="E282" t="n">
+        <v>25</v>
+      </c>
+      <c r="F282" t="n">
+        <v>13</v>
+      </c>
+      <c r="G282" t="n">
+        <v>7328</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B283" t="inlineStr">
+        <is>
+          <t>Роскачество вышло на рынок строительного...</t>
+        </is>
+      </c>
+      <c r="C283" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156990252331053</t>
+        </is>
+      </c>
+      <c r="D283" t="n">
+        <v>25</v>
+      </c>
+      <c r="E283" t="n">
+        <v>1</v>
+      </c>
+      <c r="F283" t="n">
+        <v>1</v>
+      </c>
+      <c r="G283" t="n">
+        <v>4007</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B284" t="inlineStr">
+        <is>
+          <t>Совсем скоро придет время навести порядок в...</t>
+        </is>
+      </c>
+      <c r="C284" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156990680150061</t>
+        </is>
+      </c>
+      <c r="D284" t="n">
+        <v>38</v>
+      </c>
+      <c r="E284" t="n">
+        <v>4</v>
+      </c>
+      <c r="F284" t="n">
+        <v>8</v>
+      </c>
+      <c r="G284" t="n">
+        <v>10473</v>
+      </c>
+    </row>
+    <row r="285">
+      <c r="A285" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B285" t="inlineStr">
+        <is>
+          <t>Театральный сезон уже начался: новые спектакли...</t>
+        </is>
+      </c>
+      <c r="C285" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156991164002349</t>
+        </is>
+      </c>
+      <c r="D285" t="n">
+        <v>18</v>
+      </c>
+      <c r="E285" t="n">
+        <v>0</v>
+      </c>
+      <c r="F285" t="n">
+        <v>3</v>
+      </c>
+      <c r="G285" t="n">
+        <v>3666</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B286" t="inlineStr">
+        <is>
+          <t>После длительного использования телефон часто...</t>
+        </is>
+      </c>
+      <c r="C286" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156993745006637</t>
+        </is>
+      </c>
+      <c r="D286" t="n">
+        <v>107</v>
+      </c>
+      <c r="E286" t="n">
+        <v>13</v>
+      </c>
+      <c r="F286" t="n">
+        <v>34</v>
+      </c>
+      <c r="G286" t="n">
+        <v>15896</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B287" t="inlineStr">
+        <is>
+          <t>Друзья! Совсем скоро весь мир будет отмечать...</t>
+        </is>
+      </c>
+      <c r="C287" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/156997458014253</t>
+        </is>
+      </c>
+      <c r="D287" t="n">
+        <v>25</v>
+      </c>
+      <c r="E287" t="n">
+        <v>0</v>
+      </c>
+      <c r="F287" t="n">
+        <v>2</v>
+      </c>
+      <c r="G287" t="n">
+        <v>3465</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B288" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Выбираем в магазине качественную томатную...</t>
+        </is>
+      </c>
+      <c r="C288" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/157000778395693</t>
+        </is>
+      </c>
+      <c r="D288" t="n">
+        <v>69</v>
+      </c>
+      <c r="E288" t="n">
+        <v>4</v>
+      </c>
+      <c r="F288" t="n">
+        <v>4</v>
+      </c>
+      <c r="G288" t="n">
+        <v>4747</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B289" t="inlineStr">
+        <is>
+          <t>Творожный сыр воспринимается как полезный...</t>
+        </is>
+      </c>
+      <c r="C289" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/57524942143533/topic/157002175426605</t>
+        </is>
+      </c>
+      <c r="D289" t="n">
+        <v>19</v>
+      </c>
+      <c r="E289" t="n">
+        <v>10</v>
+      </c>
+      <c r="F289" t="n">
+        <v>2</v>
+      </c>
+      <c r="G289" s="9" t="n">
+        <v>2076</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -28230,7 +30310,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G155"/>
+  <dimension ref="A1:G181"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:G1"/>
@@ -32320,6 +34400,740 @@
         <v>2592</v>
       </c>
     </row>
+    <row r="156">
+      <c r="A156" s="7" t="n"/>
+      <c r="B156" s="7" t="n"/>
+      <c r="C156" s="7" t="n"/>
+      <c r="D156" s="7" t="n"/>
+      <c r="E156" s="7" t="n"/>
+      <c r="F156" s="7" t="n"/>
+      <c r="G156" s="7" t="n"/>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>11.09.2023</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>Профессиональная оценка вина по стобалльной шкале...</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/156993735602350</t>
+        </is>
+      </c>
+      <c r="D157" s="9" t="n">
+        <v>6</v>
+      </c>
+      <c r="E157" t="n">
+        <v>0</v>
+      </c>
+      <c r="F157" t="n">
+        <v>0</v>
+      </c>
+      <c r="G157" t="n">
+        <v>3431</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>13.09.2023</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>Рубрика #рецепты к Дню шарлотки и осенних пирогов...</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157000054517934</t>
+        </is>
+      </c>
+      <c r="D158" t="n">
+        <v>17</v>
+      </c>
+      <c r="E158" t="n">
+        <v>0</v>
+      </c>
+      <c r="F158" t="n">
+        <v>6</v>
+      </c>
+      <c r="G158" t="n">
+        <v>3266</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>14.09.2023</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>Роскачество исследовало сыр в составе пицц...</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157003530809518</t>
+        </is>
+      </c>
+      <c r="D159" t="n">
+        <v>11</v>
+      </c>
+      <c r="E159" t="n">
+        <v>0</v>
+      </c>
+      <c r="F159" t="n">
+        <v>3</v>
+      </c>
+      <c r="G159" t="n">
+        <v>2957</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>15.09.2023</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>Завершающий день этапа дегустации...Цифры:..</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157006514794670</t>
+        </is>
+      </c>
+      <c r="D160" t="n">
+        <v>9</v>
+      </c>
+      <c r="E160" t="n">
+        <v>0</v>
+      </c>
+      <c r="F160" t="n">
+        <v>0</v>
+      </c>
+      <c r="G160" t="n">
+        <v>3892</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>18.09.2023</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>Эксперты «Винного гида России» выявили...</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157015147131054</t>
+        </is>
+      </c>
+      <c r="D161" t="n">
+        <v>16</v>
+      </c>
+      <c r="E161" t="n">
+        <v>4</v>
+      </c>
+      <c r="F161" t="n">
+        <v>13</v>
+      </c>
+      <c r="G161" t="n">
+        <v>8855</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>18.09.2023</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>День запахов пряностей для глинтвейна ...</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157015972950190</t>
+        </is>
+      </c>
+      <c r="D162" t="n">
+        <v>18</v>
+      </c>
+      <c r="E162" t="n">
+        <v>2</v>
+      </c>
+      <c r="F162" t="n">
+        <v>1</v>
+      </c>
+      <c r="G162" t="n">
+        <v>3274</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>19.09.2023</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>Эксперты «Винного гида России» озвучили итоги...</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157019161669806</t>
+        </is>
+      </c>
+      <c r="D163" t="n">
+        <v>11</v>
+      </c>
+      <c r="E163" t="n">
+        <v>2</v>
+      </c>
+      <c r="F163" t="n">
+        <v>0</v>
+      </c>
+      <c r="G163" t="n">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>20.09.2023</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>Вкусные #рецепты в День риса ...</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157021867520174</t>
+        </is>
+      </c>
+      <c r="D164" t="n">
+        <v>14</v>
+      </c>
+      <c r="E164" t="n">
+        <v>0</v>
+      </c>
+      <c r="F164" t="n">
+        <v>3</v>
+      </c>
+      <c r="G164" t="n">
+        <v>1929</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>21.09.2023</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Зуйкова Мария - сооснователь и винодел проекта...</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157025598746798</t>
+        </is>
+      </c>
+      <c r="D165" t="n">
+        <v>12</v>
+      </c>
+      <c r="E165" t="n">
+        <v>0</v>
+      </c>
+      <c r="F165" t="n">
+        <v>0</v>
+      </c>
+      <c r="G165" t="n">
+        <v>1352</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>22.09.2023</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>Продолжаем делиться материалами с #аудитвиноделен...</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157027914068142</t>
+        </is>
+      </c>
+      <c r="D166" t="n">
+        <v>11</v>
+      </c>
+      <c r="E166" t="n">
+        <v>0</v>
+      </c>
+      <c r="F166" t="n">
+        <v>0</v>
+      </c>
+      <c r="G166" t="n">
+        <v>1280</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>24.09.2023</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>#новостивинногомира...</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157033725997230</t>
+        </is>
+      </c>
+      <c r="D167" t="n">
+        <v>14</v>
+      </c>
+      <c r="E167" t="n">
+        <v>0</v>
+      </c>
+      <c r="F167" t="n">
+        <v>0</v>
+      </c>
+      <c r="G167" t="n">
+        <v>3422</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>25.09.2023</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>Друзья! Мы запускаем конкурс совместно с...</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157036559839406</t>
+        </is>
+      </c>
+      <c r="D168" s="8" t="n">
+        <v>222</v>
+      </c>
+      <c r="E168" s="8" t="n">
+        <v>631</v>
+      </c>
+      <c r="F168" s="8" t="n">
+        <v>92</v>
+      </c>
+      <c r="G168" s="8" t="n">
+        <v>9489</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>26.09.2023</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>В рубрике #рецепты сочетаем азиатскую лапшу с...</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157040317149358</t>
+        </is>
+      </c>
+      <c r="D169" t="n">
+        <v>63</v>
+      </c>
+      <c r="E169" t="n">
+        <v>0</v>
+      </c>
+      <c r="F169" t="n">
+        <v>10</v>
+      </c>
+      <c r="G169" t="n">
+        <v>3505</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>27.09.2023</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>Эксперты «Винного гида России» подвели итоги...</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157043602010286</t>
+        </is>
+      </c>
+      <c r="D170" t="n">
+        <v>13</v>
+      </c>
+      <c r="E170" t="n">
+        <v>0</v>
+      </c>
+      <c r="F170" t="n">
+        <v>11</v>
+      </c>
+      <c r="G170" t="n">
+        <v>4310</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>28.09.2023</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Леон Давыдов - владелец и главный винодел...</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157046205296814</t>
+        </is>
+      </c>
+      <c r="D171" t="n">
+        <v>13</v>
+      </c>
+      <c r="E171" t="n">
+        <v>0</v>
+      </c>
+      <c r="F171" t="n">
+        <v>0</v>
+      </c>
+      <c r="G171" s="9" t="n">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>01.10.2023</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Рисовая водка или рисовое вино? ...</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157055666270382</t>
+        </is>
+      </c>
+      <c r="D172" t="n">
+        <v>23</v>
+      </c>
+      <c r="E172" t="n">
+        <v>0</v>
+      </c>
+      <c r="F172" t="n">
+        <v>0</v>
+      </c>
+      <c r="G172" t="n">
+        <v>1945</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>02.10.2023</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>Во время посещения «Дней ритейла в Приморье»...</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157058920788142</t>
+        </is>
+      </c>
+      <c r="D173" t="n">
+        <v>15</v>
+      </c>
+      <c r="E173" t="n">
+        <v>2</v>
+      </c>
+      <c r="F173" t="n">
+        <v>1</v>
+      </c>
+      <c r="G173" t="n">
+        <v>2685</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>Качеству зарубежных вин стали доверять меньше. ...</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157061776191662</t>
+        </is>
+      </c>
+      <c r="D174" t="n">
+        <v>9</v>
+      </c>
+      <c r="E174" t="n">
+        <v>0</v>
+      </c>
+      <c r="F174" t="n">
+        <v>1</v>
+      </c>
+      <c r="G174" t="n">
+        <v>3620</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>Дни российских вин...</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157062509473966</t>
+        </is>
+      </c>
+      <c r="D175" t="n">
+        <v>7</v>
+      </c>
+      <c r="E175" t="n">
+        <v>0</v>
+      </c>
+      <c r="F175" t="n">
+        <v>0</v>
+      </c>
+      <c r="G175" t="n">
+        <v>2133</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>04.10.2023</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>Готовим куриный паштет к вину в рубрике...</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157065598644398</t>
+        </is>
+      </c>
+      <c r="D176" t="n">
+        <v>12</v>
+      </c>
+      <c r="E176" t="n">
+        <v>0</v>
+      </c>
+      <c r="F176" t="n">
+        <v>5</v>
+      </c>
+      <c r="G176" t="n">
+        <v>1303</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>06.10.2023</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>Подборка к Дню оранжевого вина..</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157071086629038</t>
+        </is>
+      </c>
+      <c r="D177" t="n">
+        <v>16</v>
+      </c>
+      <c r="E177" t="n">
+        <v>0</v>
+      </c>
+      <c r="F177" t="n">
+        <v>1</v>
+      </c>
+      <c r="G177" t="n">
+        <v>2477</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> К Дню почты выпустили для вас вторую серию...</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157081543618734</t>
+        </is>
+      </c>
+      <c r="D178" t="n">
+        <v>13</v>
+      </c>
+      <c r="E178" t="n">
+        <v>2</v>
+      </c>
+      <c r="F178" t="n">
+        <v>7</v>
+      </c>
+      <c r="G178" t="n">
+        <v>7031</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>А у вас еще остались подаренные и забытые кабачки...</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157084401512622</t>
+        </is>
+      </c>
+      <c r="D179" t="n">
+        <v>31</v>
+      </c>
+      <c r="E179" t="n">
+        <v>0</v>
+      </c>
+      <c r="F179" t="n">
+        <v>3</v>
+      </c>
+      <c r="G179" t="n">
+        <v>2812</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>Пользователи сайта Роскачества рекомендуют! . ..</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157090650173614</t>
+        </is>
+      </c>
+      <c r="D180" t="n">
+        <v>15</v>
+      </c>
+      <c r="E180" t="n">
+        <v>0</v>
+      </c>
+      <c r="F180" t="n">
+        <v>0</v>
+      </c>
+      <c r="G180" t="n">
+        <v>4249</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>В блогах и даже по телевизору все чаще можно...</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>https://ok.ru/group/56132723015854/topic/157092945703086</t>
+        </is>
+      </c>
+      <c r="D181" t="n">
+        <v>9</v>
+      </c>
+      <c r="E181" t="n">
+        <v>3</v>
+      </c>
+      <c r="F181" t="n">
+        <v>18</v>
+      </c>
+      <c r="G181" t="n">
+        <v>1267</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -32331,7 +35145,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I195"/>
+  <dimension ref="A1:I220"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1:I1"/>
@@ -38690,6 +41504,859 @@
         <v>58</v>
       </c>
     </row>
+    <row r="196">
+      <c r="A196" s="7" t="n"/>
+      <c r="B196" s="7" t="n"/>
+      <c r="C196" s="7" t="n"/>
+      <c r="D196" s="7" t="n"/>
+      <c r="E196" s="7" t="n"/>
+      <c r="F196" s="7" t="n"/>
+      <c r="G196" s="7" t="n"/>
+      <c r="H196" s="7" t="n"/>
+      <c r="I196" s="7" t="n"/>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>21.09.2023</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Зуйкова Мария - сооснователь и винодел проекта D</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_17258</t>
+        </is>
+      </c>
+      <c r="D197" t="n">
+        <v>156</v>
+      </c>
+      <c r="E197" t="n">
+        <v>71</v>
+      </c>
+      <c r="F197" t="n">
+        <v>4</v>
+      </c>
+      <c r="G197" t="n">
+        <v>2740</v>
+      </c>
+      <c r="H197" t="n">
+        <v>0</v>
+      </c>
+      <c r="I197" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>22.09.2023</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Продолжаем делиться материалами с #аудитвиноделен </t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_17368</t>
+        </is>
+      </c>
+      <c r="D198" t="n">
+        <v>137</v>
+      </c>
+      <c r="E198" t="n">
+        <v>58</v>
+      </c>
+      <c r="F198" t="n">
+        <v>3</v>
+      </c>
+      <c r="G198" t="n">
+        <v>1953</v>
+      </c>
+      <c r="H198" t="n">
+        <v>0</v>
+      </c>
+      <c r="I198" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>24.09.2023</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>#новостивинногомира Второй Российский винодельч</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_17463</t>
+        </is>
+      </c>
+      <c r="D199" t="n">
+        <v>196</v>
+      </c>
+      <c r="E199" t="n">
+        <v>56</v>
+      </c>
+      <c r="F199" t="n">
+        <v>2</v>
+      </c>
+      <c r="G199" t="n">
+        <v>2421</v>
+      </c>
+      <c r="H199" t="n">
+        <v>0</v>
+      </c>
+      <c r="I199" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>25.09.2023</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>Руководитель «Винного Гида России» Олеся Буняева с</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_17536</t>
+        </is>
+      </c>
+      <c r="D200" t="n">
+        <v>164</v>
+      </c>
+      <c r="E200" t="n">
+        <v>39</v>
+      </c>
+      <c r="F200" t="n">
+        <v>1</v>
+      </c>
+      <c r="G200" t="n">
+        <v>2737</v>
+      </c>
+      <c r="H200" t="n">
+        <v>1</v>
+      </c>
+      <c r="I200" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>26.09.2023</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>В рубрике #рецепты сочетаем азиатскую лапшу с росс</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_17588</t>
+        </is>
+      </c>
+      <c r="D201" t="n">
+        <v>216</v>
+      </c>
+      <c r="E201" t="n">
+        <v>52</v>
+      </c>
+      <c r="F201" t="n">
+        <v>13</v>
+      </c>
+      <c r="G201" t="n">
+        <v>2553</v>
+      </c>
+      <c r="H201" t="n">
+        <v>0</v>
+      </c>
+      <c r="I201" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>27.09.2023</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>Эксперты «Винного гида России» подвели итоги аудит</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18108</t>
+        </is>
+      </c>
+      <c r="D202" t="n">
+        <v>187</v>
+      </c>
+      <c r="E202" t="n">
+        <v>41</v>
+      </c>
+      <c r="F202" t="n">
+        <v>6</v>
+      </c>
+      <c r="G202" t="n">
+        <v>3537</v>
+      </c>
+      <c r="H202" t="n">
+        <v>2</v>
+      </c>
+      <c r="I202" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>28.09.2023</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Леон Давыдов - владелец и главный винодел “Агрол</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18316</t>
+        </is>
+      </c>
+      <c r="D203" t="n">
+        <v>113</v>
+      </c>
+      <c r="E203" t="n">
+        <v>41</v>
+      </c>
+      <c r="F203" t="n">
+        <v>1</v>
+      </c>
+      <c r="G203" t="n">
+        <v>2117</v>
+      </c>
+      <c r="H203" t="n">
+        <v>0</v>
+      </c>
+      <c r="I203" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>29.09.2023</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>«Уроки французского» к Дню учителя. Дарим1 мест</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18352</t>
+        </is>
+      </c>
+      <c r="D204" s="8" t="n">
+        <v>1413</v>
+      </c>
+      <c r="E204" s="8" t="n">
+        <v>537</v>
+      </c>
+      <c r="F204" s="8" t="n">
+        <v>403</v>
+      </c>
+      <c r="G204" s="8" t="n">
+        <v>24038</v>
+      </c>
+      <c r="H204" s="8" t="n">
+        <v>35</v>
+      </c>
+      <c r="I204" s="8" t="n">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>30.09.2023</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>День подкастов отмечается ежегодно 30 сентября.</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18488</t>
+        </is>
+      </c>
+      <c r="D205" t="n">
+        <v>85</v>
+      </c>
+      <c r="E205" t="n">
+        <v>32</v>
+      </c>
+      <c r="F205" t="n">
+        <v>1</v>
+      </c>
+      <c r="G205" t="n">
+        <v>1880</v>
+      </c>
+      <c r="H205" t="n">
+        <v>0</v>
+      </c>
+      <c r="I205" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>01.10.2023</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> Рисовая водка или рисовое вино?  Разбираемся </t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18525</t>
+        </is>
+      </c>
+      <c r="D206" t="n">
+        <v>104</v>
+      </c>
+      <c r="E206" t="n">
+        <v>50</v>
+      </c>
+      <c r="F206" t="n">
+        <v>1</v>
+      </c>
+      <c r="G206" t="n">
+        <v>1685</v>
+      </c>
+      <c r="H206" t="n">
+        <v>0</v>
+      </c>
+      <c r="I206" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>02.10.2023</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>Во время посещения «Дней ритейла в Приморье» загля</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18582</t>
+        </is>
+      </c>
+      <c r="D207" t="n">
+        <v>121</v>
+      </c>
+      <c r="E207" t="n">
+        <v>66</v>
+      </c>
+      <c r="F207" t="n">
+        <v>0</v>
+      </c>
+      <c r="G207" t="n">
+        <v>2660</v>
+      </c>
+      <c r="H207" t="n">
+        <v>0</v>
+      </c>
+      <c r="I207" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Качеству зарубежных вин стали доверять меньше. </t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18703</t>
+        </is>
+      </c>
+      <c r="D208" t="n">
+        <v>124</v>
+      </c>
+      <c r="E208" t="n">
+        <v>51</v>
+      </c>
+      <c r="F208" t="n">
+        <v>1</v>
+      </c>
+      <c r="G208" t="n">
+        <v>2067</v>
+      </c>
+      <c r="H208" t="n">
+        <v>0</v>
+      </c>
+      <c r="I208" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>03.10.2023</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>Дни российских винРады сообщить, что в рамках с</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18741</t>
+        </is>
+      </c>
+      <c r="D209" t="n">
+        <v>143</v>
+      </c>
+      <c r="E209" t="n">
+        <v>33</v>
+      </c>
+      <c r="F209" t="n">
+        <v>0</v>
+      </c>
+      <c r="G209" t="n">
+        <v>2317</v>
+      </c>
+      <c r="H209" t="n">
+        <v>0</v>
+      </c>
+      <c r="I209" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>04.10.2023</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>Готовим куриный паштет к вину в рубрике #рецепты</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_18799</t>
+        </is>
+      </c>
+      <c r="D210" t="n">
+        <v>176</v>
+      </c>
+      <c r="E210" t="n">
+        <v>42</v>
+      </c>
+      <c r="F210" t="n">
+        <v>18</v>
+      </c>
+      <c r="G210" t="n">
+        <v>3492</v>
+      </c>
+      <c r="H210" t="n">
+        <v>0</v>
+      </c>
+      <c r="I210" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>05.10.2023</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>#обзорвин
+🎦 Что такое «ледяное вино» и стоит ли его пить на свадьбе? Разбираемся на примере от [club218904093|Крымский Винный Завод]</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19175</t>
+        </is>
+      </c>
+      <c r="D211" t="n">
+        <v>124</v>
+      </c>
+      <c r="E211" t="n">
+        <v>44</v>
+      </c>
+      <c r="F211" t="n">
+        <v>4</v>
+      </c>
+      <c r="G211" t="n">
+        <v>1842</v>
+      </c>
+      <c r="H211" t="n">
+        <v>0</v>
+      </c>
+      <c r="I211" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>06.10.2023</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>Подборка к Дню оранжевого вина. А какие российс</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19240</t>
+        </is>
+      </c>
+      <c r="D212" t="n">
+        <v>109</v>
+      </c>
+      <c r="E212" t="n">
+        <v>41</v>
+      </c>
+      <c r="F212" t="n">
+        <v>10</v>
+      </c>
+      <c r="G212" t="n">
+        <v>1877</v>
+      </c>
+      <c r="H212" t="n">
+        <v>0</v>
+      </c>
+      <c r="I212" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>08.10.2023</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>#новостивинногомира  В центре энологии [club211</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19313</t>
+        </is>
+      </c>
+      <c r="D213" t="n">
+        <v>69</v>
+      </c>
+      <c r="E213" t="n">
+        <v>37</v>
+      </c>
+      <c r="F213" t="n">
+        <v>1</v>
+      </c>
+      <c r="G213" t="n">
+        <v>1750</v>
+      </c>
+      <c r="H213" t="n">
+        <v>0</v>
+      </c>
+      <c r="I213" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> К Дню почты выпустили для вас вторую серию марок</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19338</t>
+        </is>
+      </c>
+      <c r="D214" t="n">
+        <v>111</v>
+      </c>
+      <c r="E214" s="9" t="n">
+        <v>31</v>
+      </c>
+      <c r="F214" t="n">
+        <v>6</v>
+      </c>
+      <c r="G214" t="n">
+        <v>2061</v>
+      </c>
+      <c r="H214" t="n">
+        <v>0</v>
+      </c>
+      <c r="I214" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t xml:space="preserve">А у вас еще остались подаренные и забытые кабачки </t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19362</t>
+        </is>
+      </c>
+      <c r="D215" t="n">
+        <v>82</v>
+      </c>
+      <c r="E215" t="n">
+        <v>72</v>
+      </c>
+      <c r="F215" t="n">
+        <v>9</v>
+      </c>
+      <c r="G215" t="n">
+        <v>2209</v>
+      </c>
+      <c r="H215" t="n">
+        <v>0</v>
+      </c>
+      <c r="I215" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>#виннаявикторина Что за аппарат на фото и для че</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19442</t>
+        </is>
+      </c>
+      <c r="D216" t="n">
+        <v>51</v>
+      </c>
+      <c r="E216" t="n">
+        <v>44</v>
+      </c>
+      <c r="F216" t="n">
+        <v>0</v>
+      </c>
+      <c r="G216" t="n">
+        <v>2154</v>
+      </c>
+      <c r="H216" t="n">
+        <v>0</v>
+      </c>
+      <c r="I216" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Пользователи сайта Роскачества рекомендуют!  На </t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19492</t>
+        </is>
+      </c>
+      <c r="D217" t="n">
+        <v>86</v>
+      </c>
+      <c r="E217" t="n">
+        <v>34</v>
+      </c>
+      <c r="F217" t="n">
+        <v>7</v>
+      </c>
+      <c r="G217" t="n">
+        <v>1508</v>
+      </c>
+      <c r="H217" t="n">
+        <v>0</v>
+      </c>
+      <c r="I217" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>В блогах и даже по телевизору все чаще можно увиде</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19521</t>
+        </is>
+      </c>
+      <c r="D218" s="9" t="n">
+        <v>46</v>
+      </c>
+      <c r="E218" t="n">
+        <v>49</v>
+      </c>
+      <c r="F218" t="n">
+        <v>2</v>
+      </c>
+      <c r="G218" s="9" t="n">
+        <v>797</v>
+      </c>
+      <c r="H218" t="n">
+        <v>0</v>
+      </c>
+      <c r="I218" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>#обзорвин 
+Игристые новинки от [club211633726|AGORA WINERY] . Рассказываем о том, что такое</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19570</t>
+        </is>
+      </c>
+      <c r="D219" t="n">
+        <v>54</v>
+      </c>
+      <c r="E219" t="n">
+        <v>50</v>
+      </c>
+      <c r="F219" t="n">
+        <v>0</v>
+      </c>
+      <c r="G219" t="n">
+        <v>951</v>
+      </c>
+      <c r="H219" t="n">
+        <v>0</v>
+      </c>
+      <c r="I219" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>#новостивинногомира  В Краснодарском крае в ста</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>https://vk.com/wineguiderussia?w=wall-186878818_19629</t>
+        </is>
+      </c>
+      <c r="D220" t="n">
+        <v>48</v>
+      </c>
+      <c r="E220" t="n">
+        <v>50</v>
+      </c>
+      <c r="F220" t="n">
+        <v>0</v>
+      </c>
+      <c r="G220" t="n">
+        <v>952</v>
+      </c>
+      <c r="H220" t="n">
+        <v>0</v>
+      </c>
+      <c r="I220" t="n">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -38701,7 +42368,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J269"/>
+  <dimension ref="A1:J277"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
@@ -48437,6 +52104,284 @@
         <v>0</v>
       </c>
     </row>
+    <row r="270">
+      <c r="A270" s="7" t="n"/>
+      <c r="B270" s="7" t="n"/>
+      <c r="C270" s="7" t="n"/>
+      <c r="D270" s="7" t="n"/>
+      <c r="E270" s="7" t="n"/>
+      <c r="F270" s="7" t="n"/>
+      <c r="G270" s="7" t="n"/>
+      <c r="H270" s="7" t="n"/>
+      <c r="I270" s="7" t="n"/>
+      <c r="J270" s="7" t="n"/>
+    </row>
+    <row r="271">
+      <c r="A271" t="inlineStr">
+        <is>
+          <t>09.10.2023</t>
+        </is>
+      </c>
+      <c r="B271" t="inlineStr">
+        <is>
+          <t xml:space="preserve"> К Дню почты выпустили для вас вторую серию...</t>
+        </is>
+      </c>
+      <c r="C271" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2231</t>
+        </is>
+      </c>
+      <c r="D271" s="8" t="n">
+        <v>83</v>
+      </c>
+      <c r="E271" t="n">
+        <v>0</v>
+      </c>
+      <c r="F271" t="n">
+        <v>1</v>
+      </c>
+      <c r="G271" s="8" t="n">
+        <v>2</v>
+      </c>
+      <c r="H271" t="n">
+        <v>22</v>
+      </c>
+      <c r="I271" t="n">
+        <v>1643</v>
+      </c>
+      <c r="J271" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="272">
+      <c r="A272" t="inlineStr">
+        <is>
+          <t>10.10.2023</t>
+        </is>
+      </c>
+      <c r="B272" t="inlineStr">
+        <is>
+          <t>А у вас еще остались подаренные и забытые кабачки...</t>
+        </is>
+      </c>
+      <c r="C272" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2237</t>
+        </is>
+      </c>
+      <c r="D272" t="n">
+        <v>37</v>
+      </c>
+      <c r="E272" t="n">
+        <v>0</v>
+      </c>
+      <c r="F272" t="n">
+        <v>2</v>
+      </c>
+      <c r="G272" t="n">
+        <v>1</v>
+      </c>
+      <c r="H272" s="8" t="n">
+        <v>32</v>
+      </c>
+      <c r="I272" s="8" t="n">
+        <v>2397</v>
+      </c>
+      <c r="J272" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="273">
+      <c r="A273" t="inlineStr">
+        <is>
+          <t>11.10.2023</t>
+        </is>
+      </c>
+      <c r="B273" t="inlineStr">
+        <is>
+          <t>#виннаявикторина Что за аппарат на фото и для...</t>
+        </is>
+      </c>
+      <c r="C273" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2243</t>
+        </is>
+      </c>
+      <c r="D273" s="9" t="n">
+        <v>17</v>
+      </c>
+      <c r="E273" t="n">
+        <v>0</v>
+      </c>
+      <c r="F273" s="8" t="n">
+        <v>16</v>
+      </c>
+      <c r="G273" t="n">
+        <v>1</v>
+      </c>
+      <c r="H273" s="9" t="n">
+        <v>4</v>
+      </c>
+      <c r="I273" t="n">
+        <v>1779</v>
+      </c>
+      <c r="J273" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="inlineStr">
+        <is>
+          <t>12.10.2023</t>
+        </is>
+      </c>
+      <c r="B274" t="inlineStr">
+        <is>
+          <t>Пользователи сайта Роскачества рекомендуют  На...</t>
+        </is>
+      </c>
+      <c r="C274" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2245</t>
+        </is>
+      </c>
+      <c r="D274" t="n">
+        <v>36</v>
+      </c>
+      <c r="E274" t="n">
+        <v>0</v>
+      </c>
+      <c r="F274" t="n">
+        <v>2</v>
+      </c>
+      <c r="G274" t="n">
+        <v>1</v>
+      </c>
+      <c r="H274" t="n">
+        <v>19</v>
+      </c>
+      <c r="I274" s="9" t="n">
+        <v>1545</v>
+      </c>
+      <c r="J274" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="275">
+      <c r="A275" t="inlineStr">
+        <is>
+          <t>13.10.2023</t>
+        </is>
+      </c>
+      <c r="B275" t="inlineStr">
+        <is>
+          <t>В блогах и даже по телевизору все чаще можно...</t>
+        </is>
+      </c>
+      <c r="C275" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2248</t>
+        </is>
+      </c>
+      <c r="D275" t="n">
+        <v>38</v>
+      </c>
+      <c r="E275" t="n">
+        <v>0</v>
+      </c>
+      <c r="F275" t="n">
+        <v>0</v>
+      </c>
+      <c r="G275" t="n">
+        <v>0</v>
+      </c>
+      <c r="H275" t="n">
+        <v>7</v>
+      </c>
+      <c r="I275" t="n">
+        <v>1560</v>
+      </c>
+      <c r="J275" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="276">
+      <c r="A276" t="inlineStr">
+        <is>
+          <t>14.10.2023</t>
+        </is>
+      </c>
+      <c r="B276" t="inlineStr">
+        <is>
+          <t>#обзорвин  Игристые новинки от Агора Вайнери..</t>
+        </is>
+      </c>
+      <c r="C276" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2249</t>
+        </is>
+      </c>
+      <c r="D276" t="n">
+        <v>41</v>
+      </c>
+      <c r="E276" t="n">
+        <v>0</v>
+      </c>
+      <c r="F276" t="n">
+        <v>2</v>
+      </c>
+      <c r="G276" t="n">
+        <v>0</v>
+      </c>
+      <c r="H276" t="n">
+        <v>5</v>
+      </c>
+      <c r="I276" t="n">
+        <v>1736</v>
+      </c>
+      <c r="J276" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="277">
+      <c r="A277" t="inlineStr">
+        <is>
+          <t>15.10.2023</t>
+        </is>
+      </c>
+      <c r="B277" t="inlineStr">
+        <is>
+          <t>#новостивинногомира  В Краснодарском крае в...</t>
+        </is>
+      </c>
+      <c r="C277" t="inlineStr">
+        <is>
+          <t>https://t.me/wine_guide_russia/2250</t>
+        </is>
+      </c>
+      <c r="D277" t="n">
+        <v>41</v>
+      </c>
+      <c r="E277" t="n">
+        <v>0</v>
+      </c>
+      <c r="F277" t="n">
+        <v>0</v>
+      </c>
+      <c r="G277" t="n">
+        <v>1</v>
+      </c>
+      <c r="H277" t="n">
+        <v>11</v>
+      </c>
+      <c r="I277" t="n">
+        <v>1849</v>
+      </c>
+      <c r="J277" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>